<commit_message>
Dashboard and all updates
</commit_message>
<xml_diff>
--- a/server/income_details.xlsx
+++ b/server/income_details.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -425,9 +425,64 @@
         <v>45817.54185799768</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Salaryy</v>
+      </c>
+      <c r="B3">
+        <v>1500</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45817.54185799768</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Sdhjbsfryy</v>
+      </c>
+      <c r="B4">
+        <v>15000</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45817.54185799768</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>groceries</v>
+      </c>
+      <c r="B5">
+        <v>15000</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45817.54185799768</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>maid</v>
+      </c>
+      <c r="B6">
+        <v>15000</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45817.54185799768</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>jygvhcfxcgjv</v>
+      </c>
+      <c r="B7">
+        <v>1500</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45817.54185799768</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>